<commit_message>
Update functions & vignettes
</commit_message>
<xml_diff>
--- a/data-raw/functionsTracker_20230710.xlsx
+++ b/data-raw/functionsTracker_20230710.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$KL$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$KM$60</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="463">
   <si>
     <t>function</t>
   </si>
@@ -1411,6 +1411,12 @@
   <si>
     <t>*grid / *base / ggplot2</t>
   </si>
+  <si>
+    <t>vctrs</t>
+  </si>
+  <si>
+    <t>list_drop_empty</t>
+  </si>
 </sst>
 </file>
 
@@ -1762,13 +1768,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:KN60"/>
+  <dimension ref="A1:KO60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="EH34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="GX4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="HT2" sqref="HT2"/>
+      <selection pane="bottomRight" activeCell="HG4" sqref="HG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1982,91 +1988,92 @@
     <col min="212" max="212" width="6.36328125" bestFit="1" customWidth="1"/>
     <col min="213" max="213" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="214" max="214" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="215" max="215" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="6.36328125" customWidth="1"/>
-    <col min="220" max="220" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="6.6328125" customWidth="1"/>
-    <col min="226" max="226" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="6.6328125" customWidth="1"/>
-    <col min="230" max="230" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="231" max="231" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="232" max="232" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="233" max="234" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="235" max="235" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="237" max="237" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="239" max="239" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="240" max="240" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="241" max="241" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="244" max="244" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="245" max="245" width="10" customWidth="1"/>
-    <col min="246" max="246" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="249" max="249" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="250" max="250" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="252" max="252" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="253" max="253" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="254" max="254" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="18.54296875" customWidth="1"/>
-    <col min="260" max="260" width="16.453125" customWidth="1"/>
-    <col min="261" max="261" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="269" max="269" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="275" max="275" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="279" max="279" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="280" max="280" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="281" max="281" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="282" max="282" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="283" max="283" width="4.54296875" bestFit="1" customWidth="1"/>
-    <col min="284" max="284" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="285" max="285" width="6.90625" customWidth="1"/>
-    <col min="286" max="286" width="6.6328125" customWidth="1"/>
-    <col min="287" max="287" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="288" max="288" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="289" max="289" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="290" max="290" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="291" max="291" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="292" max="292" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="293" max="293" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="294" max="294" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="295" max="295" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="296" max="296" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="297" max="297" width="6" bestFit="1" customWidth="1"/>
+    <col min="215" max="215" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="217" max="217" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="219" max="219" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="220" max="220" width="6.36328125" customWidth="1"/>
+    <col min="221" max="221" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="225" max="225" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="6.6328125" customWidth="1"/>
+    <col min="227" max="227" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="6.6328125" customWidth="1"/>
+    <col min="231" max="231" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="232" max="232" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="233" max="233" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="234" max="235" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="236" max="236" width="5.08984375" bestFit="1" customWidth="1"/>
+    <col min="237" max="237" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="239" max="239" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="240" max="240" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="241" max="241" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="242" max="242" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="243" max="243" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="244" max="244" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="245" max="245" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="246" max="246" width="10" customWidth="1"/>
+    <col min="247" max="247" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="249" max="249" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="250" max="250" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="251" max="251" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="252" max="252" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="253" max="253" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="254" max="254" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="256" max="256" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="18.54296875" customWidth="1"/>
+    <col min="261" max="261" width="16.453125" customWidth="1"/>
+    <col min="262" max="262" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="265" max="265" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="268" max="268" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="272" max="272" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="273" max="273" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="274" max="274" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="275" max="275" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="276" max="276" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="277" max="277" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="279" max="279" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="281" max="281" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="282" max="282" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="283" max="283" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="284" max="284" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="285" max="285" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="286" max="286" width="6.90625" customWidth="1"/>
+    <col min="287" max="287" width="6.6328125" customWidth="1"/>
+    <col min="288" max="288" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="289" max="289" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="290" max="290" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="291" max="291" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="292" max="292" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="293" max="293" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="294" max="294" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="295" max="295" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="296" max="296" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="297" max="297" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="298" max="298" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:298" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:299" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D1" s="7" t="s">
         <v>20</v>
       </c>
@@ -2368,8 +2375,9 @@
       <c r="KJ1" s="7"/>
       <c r="KK1" s="7"/>
       <c r="KL1" s="7"/>
+      <c r="KM1" s="7"/>
     </row>
-    <row r="2" spans="1:298" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:299" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -2841,125 +2849,125 @@
       <c r="HF2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="HG2" s="4" t="s">
+      <c r="HG2" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="HH2" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="HH2" s="3" t="s">
+      <c r="HI2" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="HI2" s="4" t="s">
+      <c r="HJ2" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="HJ2" s="3" t="s">
+      <c r="HK2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="HK2" s="4" t="s">
+      <c r="HL2" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="HL2" s="3" t="s">
+      <c r="HM2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="HM2" s="4" t="s">
+      <c r="HN2" s="4" t="s">
         <v>438</v>
-      </c>
-      <c r="HN2" s="3" t="s">
-        <v>396</v>
       </c>
       <c r="HO2" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="HP2" s="4" t="s">
+      <c r="HP2" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="HQ2" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="HQ2" s="4" t="s">
+      <c r="HR2" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="HR2" s="3" t="s">
+      <c r="HS2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="HS2" s="4" t="s">
+      <c r="HT2" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="HT2" s="4" t="s">
+      <c r="HU2" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="HU2" s="4" t="s">
+      <c r="HV2" s="4" t="s">
         <v>439</v>
-      </c>
-      <c r="HV2" s="3" t="s">
-        <v>393</v>
       </c>
       <c r="HW2" s="3" t="s">
         <v>393</v>
       </c>
       <c r="HX2" s="3" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="HY2" s="3" t="s">
         <v>401</v>
       </c>
       <c r="HZ2" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="IA2" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="IA2" s="3" t="s">
+      <c r="IB2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="IB2" s="3" t="s">
+      <c r="IC2" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="IC2" s="4" t="s">
+      <c r="ID2" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="ID2" s="3" t="s">
+      <c r="IE2" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="IE2" s="4" t="s">
+      <c r="IF2" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="IF2" s="3" t="s">
+      <c r="IG2" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="IG2" s="4" t="s">
+      <c r="IH2" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="IH2" s="3" t="s">
+      <c r="II2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="II2" s="3" t="s">
+      <c r="IJ2" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="IJ2" s="3" t="s">
+      <c r="IK2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="IK2" s="3" t="s">
+      <c r="IL2" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="IL2" s="6" t="s">
+      <c r="IM2" s="6" t="s">
         <v>435</v>
-      </c>
-      <c r="IM2" s="3" t="s">
-        <v>393</v>
       </c>
       <c r="IN2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="IO2" s="4" t="s">
+      <c r="IO2" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="IP2" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="IP2" s="3" t="s">
+      <c r="IQ2" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="IQ2" s="3" t="s">
+      <c r="IR2" s="3" t="s">
         <v>396</v>
-      </c>
-      <c r="IR2" s="3" t="s">
-        <v>393</v>
       </c>
       <c r="IS2" s="3" t="s">
         <v>393</v>
       </c>
       <c r="IT2" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="IU2" s="3" t="s">
         <v>397</v>
@@ -2982,44 +2990,44 @@
       <c r="JA2" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="JB2" s="4" t="s">
+      <c r="JB2" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="JC2" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="JC2" s="3" t="s">
+      <c r="JD2" s="3" t="s">
         <v>401</v>
-      </c>
-      <c r="JD2" s="3" t="s">
-        <v>393</v>
       </c>
       <c r="JE2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="JF2" s="4" t="s">
+      <c r="JF2" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="JG2" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="JG2" s="3" t="s">
+      <c r="JH2" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="JH2" s="3" t="s">
+      <c r="JI2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="JI2" s="6" t="s">
+      <c r="JJ2" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="JJ2" s="3" t="s">
+      <c r="JK2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="JK2" s="3" t="s">
+      <c r="JL2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="JL2" s="4" t="s">
+      <c r="JM2" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="JM2" s="3" t="s">
+      <c r="JN2" s="3" t="s">
         <v>409</v>
-      </c>
-      <c r="JN2" s="3" t="s">
-        <v>410</v>
       </c>
       <c r="JO2" s="3" t="s">
         <v>410</v>
@@ -3031,70 +3039,73 @@
         <v>410</v>
       </c>
       <c r="JR2" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="JS2" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="JS2" s="4" t="s">
+      <c r="JT2" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="JT2" s="3" t="s">
+      <c r="JU2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="JU2" s="4" t="s">
+      <c r="JV2" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="JV2" s="3" t="s">
+      <c r="JW2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="JW2" s="4" t="s">
+      <c r="JX2" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="JX2" s="3" t="s">
+      <c r="JY2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="JY2" s="4" t="s">
+      <c r="JZ2" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="JZ2" s="4" t="s">
+      <c r="KA2" s="4" t="s">
         <v>427</v>
-      </c>
-      <c r="KA2" s="3" t="s">
-        <v>397</v>
       </c>
       <c r="KB2" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="KC2" s="4" t="s">
+      <c r="KC2" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="KD2" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="KD2" s="3" t="s">
+      <c r="KE2" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="KE2" s="4" t="s">
+      <c r="KF2" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="KF2" s="4" t="s">
+      <c r="KG2" s="4" t="s">
         <v>460</v>
-      </c>
-      <c r="KG2" s="3" t="s">
-        <v>393</v>
       </c>
       <c r="KH2" s="3" t="s">
         <v>393</v>
       </c>
       <c r="KI2" s="3" t="s">
-        <v>69</v>
+        <v>393</v>
       </c>
       <c r="KJ2" s="3" t="s">
         <v>69</v>
       </c>
       <c r="KK2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="KL2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="KL2" s="6" t="s">
+      <c r="KM2" s="6" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="3" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>263</v>
       </c>
@@ -3738,259 +3749,262 @@
         <v>145</v>
       </c>
       <c r="HG3" t="s">
+        <v>462</v>
+      </c>
+      <c r="HH3" t="s">
         <v>129</v>
       </c>
-      <c r="HH3" t="s">
+      <c r="HI3" t="s">
         <v>276</v>
       </c>
-      <c r="HI3" t="s">
+      <c r="HJ3" t="s">
         <v>56</v>
       </c>
-      <c r="HJ3" t="s">
+      <c r="HK3" t="s">
         <v>383</v>
       </c>
-      <c r="HK3" t="s">
+      <c r="HL3" t="s">
         <v>75</v>
       </c>
-      <c r="HL3" t="s">
+      <c r="HM3" t="s">
         <v>152</v>
       </c>
-      <c r="HM3" t="s">
+      <c r="HN3" t="s">
         <v>8</v>
       </c>
-      <c r="HN3" s="5" t="s">
+      <c r="HO3" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="HO3" s="5" t="s">
+      <c r="HP3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="HP3" t="s">
+      <c r="HQ3" t="s">
         <v>52</v>
       </c>
-      <c r="HQ3" t="s">
+      <c r="HR3" t="s">
         <v>207</v>
       </c>
-      <c r="HR3" t="s">
+      <c r="HS3" t="s">
         <v>116</v>
       </c>
-      <c r="HS3" t="s">
+      <c r="HT3" t="s">
         <v>96</v>
       </c>
-      <c r="HT3" t="s">
+      <c r="HU3" t="s">
         <v>87</v>
       </c>
-      <c r="HU3" t="s">
+      <c r="HV3" t="s">
         <v>76</v>
       </c>
-      <c r="HV3" t="s">
+      <c r="HW3" t="s">
         <v>209</v>
       </c>
-      <c r="HW3" t="s">
+      <c r="HX3" t="s">
         <v>57</v>
       </c>
-      <c r="HX3" s="5" t="s">
+      <c r="HY3" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="HY3" s="5" t="s">
+      <c r="HZ3" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="HZ3" t="s">
+      <c r="IA3" t="s">
         <v>367</v>
       </c>
-      <c r="IA3" t="s">
+      <c r="IB3" t="s">
         <v>107</v>
       </c>
-      <c r="IB3" s="5" t="s">
+      <c r="IC3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="IC3" t="s">
+      <c r="ID3" t="s">
         <v>11</v>
       </c>
-      <c r="ID3" t="s">
+      <c r="IE3" t="s">
         <v>181</v>
       </c>
-      <c r="IE3" t="s">
+      <c r="IF3" t="s">
         <v>68</v>
       </c>
-      <c r="IF3" t="s">
+      <c r="IG3" t="s">
         <v>134</v>
       </c>
-      <c r="IG3" t="s">
+      <c r="IH3" t="s">
         <v>10</v>
       </c>
-      <c r="IH3" t="s">
+      <c r="II3" t="s">
         <v>283</v>
       </c>
-      <c r="II3" t="s">
+      <c r="IJ3" t="s">
         <v>303</v>
       </c>
-      <c r="IJ3" t="s">
+      <c r="IK3" t="s">
         <v>301</v>
       </c>
-      <c r="IK3" s="5" t="s">
+      <c r="IL3" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="IL3" t="s">
+      <c r="IM3" t="s">
         <v>180</v>
       </c>
-      <c r="IM3" t="s">
+      <c r="IN3" t="s">
         <v>326</v>
       </c>
-      <c r="IN3" t="s">
+      <c r="IO3" t="s">
         <v>195</v>
       </c>
-      <c r="IO3" t="s">
+      <c r="IP3" t="s">
         <v>94</v>
       </c>
-      <c r="IP3" t="s">
+      <c r="IQ3" t="s">
         <v>74</v>
       </c>
-      <c r="IQ3" s="5" t="s">
+      <c r="IR3" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="IR3" t="s">
+      <c r="IS3" t="s">
         <v>137</v>
       </c>
-      <c r="IS3" t="s">
+      <c r="IT3" t="s">
         <v>151</v>
       </c>
-      <c r="IT3" t="s">
+      <c r="IU3" t="s">
         <v>348</v>
       </c>
-      <c r="IU3" t="s">
+      <c r="IV3" t="s">
         <v>290</v>
       </c>
-      <c r="IV3" t="s">
+      <c r="IW3" t="s">
         <v>307</v>
       </c>
-      <c r="IW3" t="s">
+      <c r="IX3" t="s">
         <v>268</v>
       </c>
-      <c r="IX3" t="s">
+      <c r="IY3" t="s">
         <v>305</v>
       </c>
-      <c r="IY3" t="s">
+      <c r="IZ3" t="s">
         <v>350</v>
       </c>
-      <c r="IZ3" t="s">
+      <c r="JA3" t="s">
         <v>269</v>
       </c>
-      <c r="JA3" t="s">
+      <c r="JB3" t="s">
         <v>270</v>
       </c>
-      <c r="JB3" t="s">
+      <c r="JC3" t="s">
         <v>5</v>
       </c>
-      <c r="JC3" s="5" t="s">
+      <c r="JD3" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="JD3" t="s">
+      <c r="JE3" t="s">
         <v>353</v>
       </c>
-      <c r="JE3" t="s">
+      <c r="JF3" t="s">
         <v>292</v>
       </c>
-      <c r="JF3" t="s">
+      <c r="JG3" t="s">
         <v>17</v>
       </c>
-      <c r="JG3" t="s">
+      <c r="JH3" t="s">
         <v>121</v>
       </c>
-      <c r="JH3" t="s">
+      <c r="JI3" t="s">
         <v>222</v>
       </c>
-      <c r="JI3" t="s">
+      <c r="JJ3" t="s">
         <v>59</v>
       </c>
-      <c r="JJ3" t="s">
+      <c r="JK3" t="s">
         <v>95</v>
       </c>
-      <c r="JK3" t="s">
+      <c r="JL3" t="s">
         <v>334</v>
       </c>
-      <c r="JL3" t="s">
+      <c r="JM3" t="s">
         <v>325</v>
       </c>
-      <c r="JM3" t="s">
+      <c r="JN3" t="s">
         <v>144</v>
       </c>
-      <c r="JN3" t="s">
+      <c r="JO3" t="s">
         <v>388</v>
       </c>
-      <c r="JO3" t="s">
+      <c r="JP3" t="s">
         <v>53</v>
       </c>
-      <c r="JP3" t="s">
+      <c r="JQ3" t="s">
         <v>392</v>
       </c>
-      <c r="JQ3" t="s">
+      <c r="JR3" t="s">
         <v>296</v>
       </c>
-      <c r="JR3" t="s">
+      <c r="JS3" t="s">
         <v>135</v>
       </c>
-      <c r="JS3" t="s">
+      <c r="JT3" t="s">
         <v>287</v>
       </c>
-      <c r="JT3" t="s">
+      <c r="JU3" t="s">
         <v>100</v>
       </c>
-      <c r="JU3" t="s">
+      <c r="JV3" t="s">
         <v>349</v>
       </c>
-      <c r="JV3" t="s">
+      <c r="JW3" t="s">
         <v>346</v>
       </c>
-      <c r="JW3" t="s">
+      <c r="JX3" t="s">
         <v>63</v>
       </c>
-      <c r="JX3" t="s">
+      <c r="JY3" t="s">
         <v>205</v>
       </c>
-      <c r="JY3" t="s">
+      <c r="JZ3" t="s">
         <v>120</v>
       </c>
-      <c r="JZ3" t="s">
+      <c r="KA3" t="s">
         <v>12</v>
       </c>
-      <c r="KA3" t="s">
+      <c r="KB3" t="s">
         <v>273</v>
       </c>
-      <c r="KB3" t="s">
+      <c r="KC3" t="s">
         <v>272</v>
       </c>
-      <c r="KC3" t="s">
+      <c r="KD3" t="s">
         <v>208</v>
       </c>
-      <c r="KD3" s="5" t="s">
+      <c r="KE3" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="KE3" t="s">
+      <c r="KF3" t="s">
         <v>6</v>
       </c>
-      <c r="KF3" t="s">
+      <c r="KG3" t="s">
         <v>277</v>
       </c>
-      <c r="KG3" t="s">
+      <c r="KH3" t="s">
         <v>80</v>
       </c>
-      <c r="KH3" t="s">
+      <c r="KI3" t="s">
         <v>206</v>
       </c>
-      <c r="KI3" t="s">
+      <c r="KJ3" t="s">
         <v>92</v>
       </c>
-      <c r="KJ3" t="s">
+      <c r="KK3" t="s">
         <v>70</v>
       </c>
-      <c r="KK3" t="s">
+      <c r="KL3" t="s">
         <v>77</v>
       </c>
-      <c r="KL3" t="s">
+      <c r="KM3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>371</v>
       </c>
@@ -4652,16 +4666,16 @@
         <v>0</v>
       </c>
       <c r="HM4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HP4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HQ4">
         <v>0</v>
@@ -4697,13 +4711,13 @@
         <v>0</v>
       </c>
       <c r="IB4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IC4">
         <v>1</v>
       </c>
       <c r="ID4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IE4">
         <v>0</v>
@@ -4712,10 +4726,10 @@
         <v>0</v>
       </c>
       <c r="IG4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II4">
         <v>0</v>
@@ -4775,10 +4789,10 @@
         <v>0</v>
       </c>
       <c r="JB4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD4">
         <v>0</v>
@@ -4787,10 +4801,10 @@
         <v>0</v>
       </c>
       <c r="JF4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JG4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JH4">
         <v>0</v>
@@ -4847,10 +4861,10 @@
         <v>0</v>
       </c>
       <c r="JZ4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KA4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KB4">
         <v>0</v>
@@ -4862,10 +4876,10 @@
         <v>0</v>
       </c>
       <c r="KE4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KF4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KG4">
         <v>0</v>
@@ -4885,8 +4899,11 @@
       <c r="KL4">
         <v>0</v>
       </c>
+      <c r="KM4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>371</v>
       </c>
@@ -5593,13 +5610,13 @@
         <v>0</v>
       </c>
       <c r="IB5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IC5">
         <v>1</v>
       </c>
       <c r="ID5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IE5">
         <v>0</v>
@@ -5608,10 +5625,10 @@
         <v>0</v>
       </c>
       <c r="IG5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II5">
         <v>0</v>
@@ -5671,10 +5688,10 @@
         <v>0</v>
       </c>
       <c r="JB5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD5">
         <v>0</v>
@@ -5683,10 +5700,10 @@
         <v>0</v>
       </c>
       <c r="JF5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JG5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JH5">
         <v>0</v>
@@ -5758,10 +5775,10 @@
         <v>0</v>
       </c>
       <c r="KE5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KF5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KG5">
         <v>0</v>
@@ -5781,8 +5798,11 @@
       <c r="KL5">
         <v>0</v>
       </c>
+      <c r="KM5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>371</v>
       </c>
@@ -6444,10 +6464,10 @@
         <v>0</v>
       </c>
       <c r="HM6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO6">
         <v>0</v>
@@ -6504,10 +6524,10 @@
         <v>0</v>
       </c>
       <c r="IG6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II6">
         <v>0</v>
@@ -6567,10 +6587,10 @@
         <v>0</v>
       </c>
       <c r="JB6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD6">
         <v>0</v>
@@ -6677,8 +6697,11 @@
       <c r="KL6">
         <v>0</v>
       </c>
+      <c r="KM6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>371</v>
       </c>
@@ -7334,10 +7357,10 @@
         <v>0</v>
       </c>
       <c r="HK7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HL7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HM7">
         <v>0</v>
@@ -7364,10 +7387,10 @@
         <v>0</v>
       </c>
       <c r="HU7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HV7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HW7">
         <v>0</v>
@@ -7427,10 +7450,10 @@
         <v>0</v>
       </c>
       <c r="IP7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IQ7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IR7">
         <v>0</v>
@@ -7463,10 +7486,10 @@
         <v>0</v>
       </c>
       <c r="JB7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD7">
         <v>0</v>
@@ -7550,31 +7573,34 @@
         <v>0</v>
       </c>
       <c r="KE7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KF7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KG7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KH7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KI7">
         <v>0</v>
       </c>
       <c r="KJ7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KK7">
         <v>1</v>
       </c>
       <c r="KL7">
+        <v>1</v>
+      </c>
+      <c r="KM7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>371</v>
       </c>
@@ -8323,10 +8349,10 @@
         <v>0</v>
       </c>
       <c r="IP8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IQ8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IR8">
         <v>0</v>
@@ -8380,10 +8406,10 @@
         <v>0</v>
       </c>
       <c r="JI8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JJ8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JK8">
         <v>0</v>
@@ -8469,8 +8495,11 @@
       <c r="KL8">
         <v>0</v>
       </c>
+      <c r="KM8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>371</v>
       </c>
@@ -9132,10 +9161,10 @@
         <v>0</v>
       </c>
       <c r="HM9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO9">
         <v>0</v>
@@ -9153,10 +9182,10 @@
         <v>0</v>
       </c>
       <c r="HT9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HU9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HV9">
         <v>0</v>
@@ -9219,10 +9248,10 @@
         <v>0</v>
       </c>
       <c r="IP9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IQ9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IR9">
         <v>0</v>
@@ -9276,10 +9305,10 @@
         <v>0</v>
       </c>
       <c r="JI9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JJ9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JK9">
         <v>0</v>
@@ -9365,8 +9394,11 @@
       <c r="KL9">
         <v>0</v>
       </c>
+      <c r="KM9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>371</v>
       </c>
@@ -10028,10 +10060,10 @@
         <v>0</v>
       </c>
       <c r="HM10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO10">
         <v>0</v>
@@ -10261,8 +10293,11 @@
       <c r="KL10">
         <v>0</v>
       </c>
+      <c r="KM10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>371</v>
       </c>
@@ -10933,10 +10968,10 @@
         <v>0</v>
       </c>
       <c r="HP11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HQ11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HR11">
         <v>0</v>
@@ -10984,10 +11019,10 @@
         <v>0</v>
       </c>
       <c r="IG11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II11">
         <v>0</v>
@@ -11017,10 +11052,10 @@
         <v>0</v>
       </c>
       <c r="IR11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IS11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IT11">
         <v>0</v>
@@ -11047,10 +11082,10 @@
         <v>0</v>
       </c>
       <c r="JB11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD11">
         <v>0</v>
@@ -11095,10 +11130,10 @@
         <v>0</v>
       </c>
       <c r="JR11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JS11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JT11">
         <v>0</v>
@@ -11157,8 +11192,11 @@
       <c r="KL11">
         <v>0</v>
       </c>
+      <c r="KM11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>371</v>
       </c>
@@ -11820,10 +11858,10 @@
         <v>0</v>
       </c>
       <c r="HM12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO12">
         <v>0</v>
@@ -11850,10 +11888,10 @@
         <v>0</v>
       </c>
       <c r="HW12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY12">
         <v>0</v>
@@ -11868,10 +11906,10 @@
         <v>0</v>
       </c>
       <c r="IC12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="ID12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IE12">
         <v>0</v>
@@ -11880,10 +11918,10 @@
         <v>0</v>
       </c>
       <c r="IG12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II12">
         <v>0</v>
@@ -11943,10 +11981,10 @@
         <v>0</v>
       </c>
       <c r="JB12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD12">
         <v>0</v>
@@ -12027,10 +12065,10 @@
         <v>0</v>
       </c>
       <c r="KD12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KE12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KF12">
         <v>0</v>
@@ -12053,8 +12091,11 @@
       <c r="KL12">
         <v>0</v>
       </c>
+      <c r="KM12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>371</v>
       </c>
@@ -12698,10 +12739,10 @@
         <v>0</v>
       </c>
       <c r="HG13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HH13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HI13">
         <v>0</v>
@@ -12716,10 +12757,10 @@
         <v>0</v>
       </c>
       <c r="HM13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO13">
         <v>0</v>
@@ -12734,10 +12775,10 @@
         <v>0</v>
       </c>
       <c r="HS13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HU13">
         <v>0</v>
@@ -12746,10 +12787,10 @@
         <v>0</v>
       </c>
       <c r="HW13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY13">
         <v>0</v>
@@ -12773,10 +12814,10 @@
         <v>0</v>
       </c>
       <c r="IF13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IG13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IH13">
         <v>0</v>
@@ -12842,10 +12883,10 @@
         <v>0</v>
       </c>
       <c r="JC13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JD13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JE13">
         <v>0</v>
@@ -12949,8 +12990,11 @@
       <c r="KL13">
         <v>0</v>
       </c>
+      <c r="KM13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>371</v>
       </c>
@@ -13630,10 +13674,10 @@
         <v>0</v>
       </c>
       <c r="HS14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HU14">
         <v>0</v>
@@ -13696,10 +13740,10 @@
         <v>0</v>
       </c>
       <c r="IO14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IP14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IQ14">
         <v>0</v>
@@ -13759,10 +13803,10 @@
         <v>0</v>
       </c>
       <c r="JJ14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JK14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JL14">
         <v>0</v>
@@ -13789,10 +13833,10 @@
         <v>0</v>
       </c>
       <c r="JT14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JU14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JV14">
         <v>0</v>
@@ -13834,10 +13878,10 @@
         <v>0</v>
       </c>
       <c r="KI14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KJ14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KK14">
         <v>0</v>
@@ -13845,8 +13889,11 @@
       <c r="KL14">
         <v>0</v>
       </c>
+      <c r="KM14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>371</v>
       </c>
@@ -14568,10 +14615,10 @@
         <v>0</v>
       </c>
       <c r="IG15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II15">
         <v>0</v>
@@ -14715,10 +14762,10 @@
         <v>0</v>
       </c>
       <c r="KD15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KE15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KF15">
         <v>0</v>
@@ -14741,8 +14788,11 @@
       <c r="KL15">
         <v>0</v>
       </c>
+      <c r="KM15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>371</v>
       </c>
@@ -15404,10 +15454,10 @@
         <v>0</v>
       </c>
       <c r="HM16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO16">
         <v>0</v>
@@ -15434,10 +15484,10 @@
         <v>0</v>
       </c>
       <c r="HW16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY16">
         <v>0</v>
@@ -15485,10 +15535,10 @@
         <v>0</v>
       </c>
       <c r="IN16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IO16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IP16">
         <v>0</v>
@@ -15581,10 +15631,10 @@
         <v>0</v>
       </c>
       <c r="JT16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JU16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JV16">
         <v>0</v>
@@ -15611,10 +15661,10 @@
         <v>0</v>
       </c>
       <c r="KD16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KE16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KF16">
         <v>0</v>
@@ -15637,8 +15687,11 @@
       <c r="KL16">
         <v>0</v>
       </c>
+      <c r="KM16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>369</v>
       </c>
@@ -16300,19 +16353,19 @@
         <v>0</v>
       </c>
       <c r="HM17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO17">
         <v>0</v>
       </c>
       <c r="HP17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HQ17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HR17">
         <v>0</v>
@@ -16345,10 +16398,10 @@
         <v>0</v>
       </c>
       <c r="IB17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IC17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ID17">
         <v>0</v>
@@ -16372,10 +16425,10 @@
         <v>0</v>
       </c>
       <c r="IK17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IL17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IM17">
         <v>0</v>
@@ -16423,10 +16476,10 @@
         <v>0</v>
       </c>
       <c r="JB17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD17">
         <v>0</v>
@@ -16456,10 +16509,10 @@
         <v>0</v>
       </c>
       <c r="JM17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JN17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JO17">
         <v>0</v>
@@ -16510,10 +16563,10 @@
         <v>0</v>
       </c>
       <c r="KE17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KF17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KG17">
         <v>0</v>
@@ -16533,8 +16586,11 @@
       <c r="KL17">
         <v>0</v>
       </c>
+      <c r="KM17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>369</v>
       </c>
@@ -17214,10 +17270,10 @@
         <v>0</v>
       </c>
       <c r="HS18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HU18">
         <v>0</v>
@@ -17238,10 +17294,10 @@
         <v>0</v>
       </c>
       <c r="IA18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IB18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IC18">
         <v>0</v>
@@ -17319,10 +17375,10 @@
         <v>0</v>
       </c>
       <c r="JB18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD18">
         <v>0</v>
@@ -17331,10 +17387,10 @@
         <v>0</v>
       </c>
       <c r="JF18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JG18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JH18">
         <v>0</v>
@@ -17429,8 +17485,11 @@
       <c r="KL18">
         <v>0</v>
       </c>
+      <c r="KM18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>369</v>
       </c>
@@ -18110,10 +18169,10 @@
         <v>0</v>
       </c>
       <c r="HS19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HU19">
         <v>0</v>
@@ -18134,10 +18193,10 @@
         <v>0</v>
       </c>
       <c r="IA19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IB19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IC19">
         <v>0</v>
@@ -18215,10 +18274,10 @@
         <v>0</v>
       </c>
       <c r="JB19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD19">
         <v>0</v>
@@ -18325,8 +18384,11 @@
       <c r="KL19">
         <v>0</v>
       </c>
+      <c r="KM19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>369</v>
       </c>
@@ -18988,10 +19050,10 @@
         <v>0</v>
       </c>
       <c r="HM20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO20">
         <v>0</v>
@@ -19006,10 +19068,10 @@
         <v>0</v>
       </c>
       <c r="HS20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HU20">
         <v>0</v>
@@ -19030,16 +19092,16 @@
         <v>0</v>
       </c>
       <c r="IA20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IB20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IC20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="ID20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IE20">
         <v>0</v>
@@ -19048,10 +19110,10 @@
         <v>0</v>
       </c>
       <c r="IG20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II20">
         <v>0</v>
@@ -19111,10 +19173,10 @@
         <v>0</v>
       </c>
       <c r="JB20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD20">
         <v>0</v>
@@ -19198,10 +19260,10 @@
         <v>0</v>
       </c>
       <c r="KE20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KF20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KG20">
         <v>0</v>
@@ -19221,8 +19283,11 @@
       <c r="KL20">
         <v>0</v>
       </c>
+      <c r="KM20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>369</v>
       </c>
@@ -19899,10 +19964,10 @@
         <v>0</v>
       </c>
       <c r="HR21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HS21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HT21">
         <v>0</v>
@@ -19926,13 +19991,13 @@
         <v>0</v>
       </c>
       <c r="IA21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IB21">
         <v>1</v>
       </c>
       <c r="IC21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ID21">
         <v>0</v>
@@ -20007,10 +20072,10 @@
         <v>0</v>
       </c>
       <c r="JB21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD21">
         <v>0</v>
@@ -20117,8 +20182,11 @@
       <c r="KL21">
         <v>0</v>
       </c>
+      <c r="KM21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>369</v>
       </c>
@@ -20762,7 +20830,7 @@
         <v>1</v>
       </c>
       <c r="HG22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HH22">
         <v>0</v>
@@ -20798,10 +20866,10 @@
         <v>0</v>
       </c>
       <c r="HS22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HU22">
         <v>0</v>
@@ -20810,10 +20878,10 @@
         <v>0</v>
       </c>
       <c r="HW22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY22">
         <v>0</v>
@@ -20822,7 +20890,7 @@
         <v>0</v>
       </c>
       <c r="IA22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IB22">
         <v>1</v>
@@ -20831,7 +20899,7 @@
         <v>1</v>
       </c>
       <c r="ID22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IE22">
         <v>0</v>
@@ -20840,10 +20908,10 @@
         <v>0</v>
       </c>
       <c r="IG22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II22">
         <v>0</v>
@@ -20903,10 +20971,10 @@
         <v>0</v>
       </c>
       <c r="JB22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD22">
         <v>0</v>
@@ -20918,16 +20986,16 @@
         <v>0</v>
       </c>
       <c r="JG22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JH22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JI22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JJ22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JK22">
         <v>0</v>
@@ -20972,10 +21040,10 @@
         <v>0</v>
       </c>
       <c r="JY22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JZ22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KA22">
         <v>0</v>
@@ -21013,8 +21081,11 @@
       <c r="KL22">
         <v>0</v>
       </c>
+      <c r="KM22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>368</v>
       </c>
@@ -21676,22 +21747,22 @@
         <v>0</v>
       </c>
       <c r="HM23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO23">
         <v>0</v>
       </c>
       <c r="HP23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HQ23">
         <v>1</v>
       </c>
       <c r="HR23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HS23">
         <v>0</v>
@@ -21703,13 +21774,13 @@
         <v>0</v>
       </c>
       <c r="HV23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HW23">
         <v>1</v>
       </c>
       <c r="HX23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY23">
         <v>0</v>
@@ -21799,10 +21870,10 @@
         <v>0</v>
       </c>
       <c r="JB23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD23">
         <v>0</v>
@@ -21880,10 +21951,10 @@
         <v>0</v>
       </c>
       <c r="KC23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KD23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KE23">
         <v>0</v>
@@ -21895,23 +21966,26 @@
         <v>0</v>
       </c>
       <c r="KH23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KI23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KJ23">
         <v>0</v>
       </c>
       <c r="KK23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KL23">
-        <v>0</v>
-      </c>
-      <c r="KN23" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="KM23">
+        <v>0</v>
+      </c>
+      <c r="KO23" s="3"/>
     </row>
-    <row r="24" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>368</v>
       </c>
@@ -22696,10 +22770,10 @@
         <v>0</v>
       </c>
       <c r="JB24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD24">
         <v>0</v>
@@ -22806,9 +22880,12 @@
       <c r="KL24">
         <v>0</v>
       </c>
-      <c r="KN24" s="3"/>
+      <c r="KM24">
+        <v>0</v>
+      </c>
+      <c r="KO24" s="3"/>
     </row>
-    <row r="25" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>368</v>
       </c>
@@ -23703,8 +23780,11 @@
       <c r="KL25">
         <v>0</v>
       </c>
+      <c r="KM25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>368</v>
       </c>
@@ -24599,8 +24679,11 @@
       <c r="KL26">
         <v>0</v>
       </c>
+      <c r="KM26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>368</v>
       </c>
@@ -25349,10 +25432,10 @@
         <v>0</v>
       </c>
       <c r="IP27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IQ27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IR27">
         <v>0</v>
@@ -25484,10 +25567,10 @@
         <v>0</v>
       </c>
       <c r="KI27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KJ27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KK27">
         <v>0</v>
@@ -25495,8 +25578,11 @@
       <c r="KL27">
         <v>0</v>
       </c>
+      <c r="KM27">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>368</v>
       </c>
@@ -26281,10 +26367,10 @@
         <v>0</v>
       </c>
       <c r="JB28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD28">
         <v>0</v>
@@ -26391,8 +26477,11 @@
       <c r="KL28">
         <v>0</v>
       </c>
+      <c r="KM28">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>368</v>
       </c>
@@ -27195,10 +27284,10 @@
         <v>0</v>
       </c>
       <c r="JH29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JI29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JJ29">
         <v>0</v>
@@ -27287,8 +27376,11 @@
       <c r="KL29">
         <v>0</v>
       </c>
+      <c r="KM29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>368</v>
       </c>
@@ -28091,10 +28183,10 @@
         <v>0</v>
       </c>
       <c r="JH30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JI30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JJ30">
         <v>0</v>
@@ -28183,8 +28275,11 @@
       <c r="KL30">
         <v>0</v>
       </c>
+      <c r="KM30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>368</v>
       </c>
@@ -28969,10 +29064,10 @@
         <v>0</v>
       </c>
       <c r="JB31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD31">
         <v>0</v>
@@ -29079,8 +29174,11 @@
       <c r="KL31">
         <v>0</v>
       </c>
+      <c r="KM31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:300" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:301" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>368</v>
       </c>
@@ -29775,10 +29873,10 @@
         <v>0</v>
       </c>
       <c r="HX32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HY32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HZ32">
         <v>0</v>
@@ -29975,8 +30073,11 @@
       <c r="KL32">
         <v>0</v>
       </c>
+      <c r="KM32">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>370</v>
       </c>
@@ -30635,10 +30736,10 @@
         <v>0</v>
       </c>
       <c r="HL33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HM33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HN33">
         <v>0</v>
@@ -30668,10 +30769,10 @@
         <v>0</v>
       </c>
       <c r="HW33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY33">
         <v>0</v>
@@ -30734,10 +30835,10 @@
         <v>0</v>
       </c>
       <c r="IS33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IT33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IU33">
         <v>0</v>
@@ -30869,10 +30970,13 @@
         <v>0</v>
       </c>
       <c r="KL33">
+        <v>0</v>
+      </c>
+      <c r="KM33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>370</v>
       </c>
@@ -31564,10 +31668,10 @@
         <v>0</v>
       </c>
       <c r="HW34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY34">
         <v>0</v>
@@ -31723,10 +31827,10 @@
         <v>0</v>
       </c>
       <c r="JX34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JY34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JZ34">
         <v>0</v>
@@ -31767,8 +31871,11 @@
       <c r="KL34">
         <v>0</v>
       </c>
+      <c r="KM34">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>128</v>
       </c>
@@ -32418,10 +32525,10 @@
         <v>0</v>
       </c>
       <c r="HI35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HJ35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HK35">
         <v>0</v>
@@ -32430,10 +32537,10 @@
         <v>0</v>
       </c>
       <c r="HM35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO35">
         <v>0</v>
@@ -32460,10 +32567,10 @@
         <v>0</v>
       </c>
       <c r="HW35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY35">
         <v>0</v>
@@ -32478,10 +32585,10 @@
         <v>0</v>
       </c>
       <c r="IC35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="ID35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IE35">
         <v>0</v>
@@ -32490,10 +32597,10 @@
         <v>0</v>
       </c>
       <c r="IG35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II35">
         <v>0</v>
@@ -32553,10 +32660,10 @@
         <v>0</v>
       </c>
       <c r="JB35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD35">
         <v>0</v>
@@ -32574,10 +32681,10 @@
         <v>0</v>
       </c>
       <c r="JI35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JJ35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JK35">
         <v>0</v>
@@ -32616,10 +32723,10 @@
         <v>0</v>
       </c>
       <c r="JW35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JX35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JY35">
         <v>0</v>
@@ -32663,8 +32770,11 @@
       <c r="KL35">
         <v>0</v>
       </c>
+      <c r="KM35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>128</v>
       </c>
@@ -33326,16 +33436,16 @@
         <v>0</v>
       </c>
       <c r="HM36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HP36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HQ36">
         <v>0</v>
@@ -33377,10 +33487,10 @@
         <v>0</v>
       </c>
       <c r="ID36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IE36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IF36">
         <v>0</v>
@@ -33449,10 +33559,10 @@
         <v>0</v>
       </c>
       <c r="JB36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD36">
         <v>0</v>
@@ -33488,10 +33598,10 @@
         <v>0</v>
       </c>
       <c r="JO36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JP36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JQ36">
         <v>0</v>
@@ -33503,10 +33613,10 @@
         <v>0</v>
       </c>
       <c r="JT36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JU36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JV36">
         <v>0</v>
@@ -33559,8 +33669,11 @@
       <c r="KL36">
         <v>0</v>
       </c>
+      <c r="KM36">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>128</v>
       </c>
@@ -34222,19 +34335,19 @@
         <v>0</v>
       </c>
       <c r="HM37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO37">
         <v>0</v>
       </c>
       <c r="HP37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HQ37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HR37">
         <v>0</v>
@@ -34273,10 +34386,10 @@
         <v>0</v>
       </c>
       <c r="ID37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IE37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IF37">
         <v>0</v>
@@ -34384,10 +34497,10 @@
         <v>0</v>
       </c>
       <c r="JO37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JP37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JQ37">
         <v>0</v>
@@ -34455,8 +34568,11 @@
       <c r="KL37">
         <v>0</v>
       </c>
+      <c r="KM37">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>128</v>
       </c>
@@ -35127,10 +35243,10 @@
         <v>0</v>
       </c>
       <c r="HP38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HQ38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HR38">
         <v>0</v>
@@ -35172,10 +35288,10 @@
         <v>0</v>
       </c>
       <c r="IE38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IF38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IG38">
         <v>0</v>
@@ -35241,10 +35357,10 @@
         <v>0</v>
       </c>
       <c r="JB38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD38">
         <v>0</v>
@@ -35280,10 +35396,10 @@
         <v>0</v>
       </c>
       <c r="JO38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JP38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JQ38">
         <v>0</v>
@@ -35351,8 +35467,11 @@
       <c r="KL38">
         <v>0</v>
       </c>
+      <c r="KM38">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>372</v>
       </c>
@@ -36143,10 +36262,10 @@
         <v>0</v>
       </c>
       <c r="JD39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JE39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JF39">
         <v>0</v>
@@ -36164,10 +36283,10 @@
         <v>0</v>
       </c>
       <c r="JK39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JL39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JM39">
         <v>0</v>
@@ -36218,10 +36337,10 @@
         <v>0</v>
       </c>
       <c r="KC39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KD39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KE39">
         <v>0</v>
@@ -36247,8 +36366,11 @@
       <c r="KL39">
         <v>0</v>
       </c>
+      <c r="KM39">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>372</v>
       </c>
@@ -37033,10 +37155,10 @@
         <v>0</v>
       </c>
       <c r="JB40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD40">
         <v>0</v>
@@ -37143,8 +37265,11 @@
       <c r="KL40">
         <v>0</v>
       </c>
+      <c r="KM40">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>372</v>
       </c>
@@ -37806,10 +37931,10 @@
         <v>0</v>
       </c>
       <c r="HM41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO41">
         <v>0</v>
@@ -37824,10 +37949,10 @@
         <v>0</v>
       </c>
       <c r="HS41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HU41">
         <v>0</v>
@@ -37854,10 +37979,10 @@
         <v>0</v>
       </c>
       <c r="IC41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="ID41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IE41">
         <v>0</v>
@@ -37881,13 +38006,13 @@
         <v>0</v>
       </c>
       <c r="IL41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IM41">
         <v>1</v>
       </c>
       <c r="IN41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IO41">
         <v>0</v>
@@ -37929,10 +38054,10 @@
         <v>0</v>
       </c>
       <c r="JB41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD41">
         <v>0</v>
@@ -37959,10 +38084,10 @@
         <v>0</v>
       </c>
       <c r="JL41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JM41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JN41">
         <v>0</v>
@@ -38010,10 +38135,10 @@
         <v>0</v>
       </c>
       <c r="KC41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KD41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KE41">
         <v>0</v>
@@ -38028,10 +38153,10 @@
         <v>0</v>
       </c>
       <c r="KI41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KJ41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KK41">
         <v>0</v>
@@ -38039,8 +38164,11 @@
       <c r="KL41">
         <v>0</v>
       </c>
+      <c r="KM41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>372</v>
       </c>
@@ -38720,10 +38848,10 @@
         <v>0</v>
       </c>
       <c r="HS42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HU42">
         <v>0</v>
@@ -38855,10 +38983,10 @@
         <v>0</v>
       </c>
       <c r="JL42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JM42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JN42">
         <v>0</v>
@@ -38935,8 +39063,11 @@
       <c r="KL42">
         <v>0</v>
       </c>
+      <c r="KM42">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>372</v>
       </c>
@@ -39721,10 +39852,10 @@
         <v>0</v>
       </c>
       <c r="JB43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD43">
         <v>0</v>
@@ -39751,10 +39882,10 @@
         <v>0</v>
       </c>
       <c r="JL43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JM43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JN43">
         <v>0</v>
@@ -39831,8 +39962,11 @@
       <c r="KL43">
         <v>0</v>
       </c>
+      <c r="KM43">
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>372</v>
       </c>
@@ -40494,10 +40628,10 @@
         <v>0</v>
       </c>
       <c r="HM44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO44">
         <v>0</v>
@@ -40569,10 +40703,10 @@
         <v>0</v>
       </c>
       <c r="IL44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IM44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IN44">
         <v>0</v>
@@ -40644,10 +40778,10 @@
         <v>0</v>
       </c>
       <c r="JK44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JL44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JM44">
         <v>0</v>
@@ -40727,8 +40861,11 @@
       <c r="KL44">
         <v>0</v>
       </c>
+      <c r="KM44">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>372</v>
       </c>
@@ -41381,19 +41518,19 @@
         <v>0</v>
       </c>
       <c r="HJ45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HK45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HL45">
         <v>0</v>
       </c>
       <c r="HM45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO45">
         <v>0</v>
@@ -41420,16 +41557,16 @@
         <v>0</v>
       </c>
       <c r="HW45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HZ45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IA45">
         <v>0</v>
@@ -41471,10 +41608,10 @@
         <v>0</v>
       </c>
       <c r="IN45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IO45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IP45">
         <v>0</v>
@@ -41513,10 +41650,10 @@
         <v>0</v>
       </c>
       <c r="JB45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD45">
         <v>0</v>
@@ -41597,10 +41734,10 @@
         <v>0</v>
       </c>
       <c r="KD45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KE45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KF45">
         <v>0</v>
@@ -41623,8 +41760,11 @@
       <c r="KL45">
         <v>0</v>
       </c>
+      <c r="KM45">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>372</v>
       </c>
@@ -42286,10 +42426,10 @@
         <v>0</v>
       </c>
       <c r="HM46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO46">
         <v>0</v>
@@ -42322,10 +42462,10 @@
         <v>0</v>
       </c>
       <c r="HY46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HZ46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IA46">
         <v>0</v>
@@ -42409,10 +42549,10 @@
         <v>0</v>
       </c>
       <c r="JB46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD46">
         <v>0</v>
@@ -42445,10 +42585,10 @@
         <v>0</v>
       </c>
       <c r="JN46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JO46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JP46">
         <v>0</v>
@@ -42519,8 +42659,11 @@
       <c r="KL46">
         <v>0</v>
       </c>
+      <c r="KM46">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>372</v>
       </c>
@@ -43182,10 +43325,10 @@
         <v>0</v>
       </c>
       <c r="HM47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO47">
         <v>0</v>
@@ -43212,16 +43355,16 @@
         <v>0</v>
       </c>
       <c r="HW47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HZ47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IA47">
         <v>0</v>
@@ -43242,10 +43385,10 @@
         <v>0</v>
       </c>
       <c r="IG47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II47">
         <v>0</v>
@@ -43263,10 +43406,10 @@
         <v>0</v>
       </c>
       <c r="IN47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IO47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IP47">
         <v>0</v>
@@ -43305,10 +43448,10 @@
         <v>0</v>
       </c>
       <c r="JB47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD47">
         <v>0</v>
@@ -43341,10 +43484,10 @@
         <v>0</v>
       </c>
       <c r="JN47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JO47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JP47">
         <v>0</v>
@@ -43415,8 +43558,11 @@
       <c r="KL47">
         <v>0</v>
       </c>
+      <c r="KM47">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>372</v>
       </c>
@@ -44078,13 +44224,13 @@
         <v>0</v>
       </c>
       <c r="HM48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN48">
         <v>1</v>
       </c>
       <c r="HO48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HP48">
         <v>0</v>
@@ -44108,16 +44254,16 @@
         <v>0</v>
       </c>
       <c r="HW48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HZ48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IA48">
         <v>0</v>
@@ -44138,10 +44284,10 @@
         <v>0</v>
       </c>
       <c r="IG48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II48">
         <v>0</v>
@@ -44159,10 +44305,10 @@
         <v>0</v>
       </c>
       <c r="IN48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IO48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IP48">
         <v>0</v>
@@ -44201,10 +44347,10 @@
         <v>0</v>
       </c>
       <c r="JB48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD48">
         <v>0</v>
@@ -44237,16 +44383,16 @@
         <v>0</v>
       </c>
       <c r="JN48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JO48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JP48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JQ48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JR48">
         <v>0</v>
@@ -44285,10 +44431,10 @@
         <v>0</v>
       </c>
       <c r="KD48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KE48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KF48">
         <v>0</v>
@@ -44311,8 +44457,11 @@
       <c r="KL48">
         <v>0</v>
       </c>
+      <c r="KM48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>372</v>
       </c>
@@ -44965,19 +45114,19 @@
         <v>0</v>
       </c>
       <c r="HJ49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HK49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HL49">
         <v>0</v>
       </c>
       <c r="HM49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO49">
         <v>0</v>
@@ -45004,16 +45153,16 @@
         <v>0</v>
       </c>
       <c r="HW49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HZ49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IA49">
         <v>0</v>
@@ -45055,10 +45204,10 @@
         <v>0</v>
       </c>
       <c r="IN49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IO49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IP49">
         <v>0</v>
@@ -45097,10 +45246,10 @@
         <v>0</v>
       </c>
       <c r="JB49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD49">
         <v>0</v>
@@ -45181,10 +45330,10 @@
         <v>0</v>
       </c>
       <c r="KD49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KE49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KF49">
         <v>0</v>
@@ -45207,8 +45356,11 @@
       <c r="KL49">
         <v>0</v>
       </c>
+      <c r="KM49">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>372</v>
       </c>
@@ -45870,10 +46022,10 @@
         <v>0</v>
       </c>
       <c r="HM50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO50">
         <v>0</v>
@@ -45888,10 +46040,10 @@
         <v>0</v>
       </c>
       <c r="HS50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HU50">
         <v>0</v>
@@ -45906,22 +46058,22 @@
         <v>0</v>
       </c>
       <c r="HY50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HZ50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IA50">
         <v>0</v>
       </c>
       <c r="IB50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IC50">
         <v>1</v>
       </c>
       <c r="ID50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IE50">
         <v>0</v>
@@ -45930,10 +46082,10 @@
         <v>0</v>
       </c>
       <c r="IG50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II50">
         <v>0</v>
@@ -45960,10 +46112,10 @@
         <v>0</v>
       </c>
       <c r="IQ50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IR50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IS50">
         <v>0</v>
@@ -45993,10 +46145,10 @@
         <v>0</v>
       </c>
       <c r="JB50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD50">
         <v>0</v>
@@ -46029,10 +46181,10 @@
         <v>0</v>
       </c>
       <c r="JN50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JO50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JP50">
         <v>0</v>
@@ -46047,10 +46199,10 @@
         <v>0</v>
       </c>
       <c r="JT50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JU50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JV50">
         <v>0</v>
@@ -46077,13 +46229,13 @@
         <v>0</v>
       </c>
       <c r="KD50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KE50">
         <v>1</v>
       </c>
       <c r="KF50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KG50">
         <v>0</v>
@@ -46103,8 +46255,11 @@
       <c r="KL50">
         <v>0</v>
       </c>
+      <c r="KM50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>372</v>
       </c>
@@ -46766,10 +46921,10 @@
         <v>0</v>
       </c>
       <c r="HM51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO51">
         <v>0</v>
@@ -46865,34 +47020,34 @@
         <v>0</v>
       </c>
       <c r="IT51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IU51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IV51">
         <v>0</v>
       </c>
       <c r="IW51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IX51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IY51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IZ51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JA51">
         <v>0</v>
       </c>
       <c r="JB51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD51">
         <v>0</v>
@@ -46946,13 +47101,13 @@
         <v>0</v>
       </c>
       <c r="JU51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JV51">
         <v>1</v>
       </c>
       <c r="JW51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JX51">
         <v>0</v>
@@ -46964,28 +47119,28 @@
         <v>0</v>
       </c>
       <c r="KA51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KB51">
         <v>1</v>
       </c>
       <c r="KC51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KD51">
         <v>0</v>
       </c>
       <c r="KE51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KF51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KG51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KH51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KI51">
         <v>0</v>
@@ -46999,8 +47154,11 @@
       <c r="KL51">
         <v>0</v>
       </c>
+      <c r="KM51">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>372</v>
       </c>
@@ -47895,8 +48053,11 @@
       <c r="KL52">
         <v>0</v>
       </c>
+      <c r="KM52">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>372</v>
       </c>
@@ -48588,19 +48749,19 @@
         <v>0</v>
       </c>
       <c r="HW53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY53">
         <v>0</v>
       </c>
       <c r="HZ53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IA53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IB53">
         <v>0</v>
@@ -48791,8 +48952,11 @@
       <c r="KL53">
         <v>0</v>
       </c>
+      <c r="KM53">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>372</v>
       </c>
@@ -49439,10 +49603,10 @@
         <v>0</v>
       </c>
       <c r="HH54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HI54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HJ54">
         <v>0</v>
@@ -49454,10 +49618,10 @@
         <v>0</v>
       </c>
       <c r="HM54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO54">
         <v>0</v>
@@ -49484,10 +49648,10 @@
         <v>0</v>
       </c>
       <c r="HW54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY54">
         <v>0</v>
@@ -49562,22 +49726,22 @@
         <v>0</v>
       </c>
       <c r="IW54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IX54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IY54">
         <v>0</v>
       </c>
       <c r="IZ54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JA54">
         <v>1</v>
       </c>
       <c r="JB54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JC54">
         <v>0</v>
@@ -49652,13 +49816,13 @@
         <v>0</v>
       </c>
       <c r="KA54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KB54">
         <v>1</v>
       </c>
       <c r="KC54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KD54">
         <v>0</v>
@@ -49667,10 +49831,10 @@
         <v>0</v>
       </c>
       <c r="KF54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KG54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KH54">
         <v>0</v>
@@ -49687,8 +49851,11 @@
       <c r="KL54">
         <v>0</v>
       </c>
+      <c r="KM54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>372</v>
       </c>
@@ -50350,10 +50517,10 @@
         <v>0</v>
       </c>
       <c r="HM55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO55">
         <v>0</v>
@@ -50368,10 +50535,10 @@
         <v>0</v>
       </c>
       <c r="HS55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HU55">
         <v>0</v>
@@ -50380,10 +50547,10 @@
         <v>0</v>
       </c>
       <c r="HW55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY55">
         <v>0</v>
@@ -50398,10 +50565,10 @@
         <v>0</v>
       </c>
       <c r="IC55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="ID55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IE55">
         <v>0</v>
@@ -50413,19 +50580,19 @@
         <v>0</v>
       </c>
       <c r="IH55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="II55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IJ55">
         <v>0</v>
       </c>
       <c r="IK55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IL55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IM55">
         <v>0</v>
@@ -50452,10 +50619,10 @@
         <v>0</v>
       </c>
       <c r="IU55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IV55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IW55">
         <v>0</v>
@@ -50473,19 +50640,19 @@
         <v>0</v>
       </c>
       <c r="JB55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD55">
         <v>0</v>
       </c>
       <c r="JE55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JF55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JG55">
         <v>0</v>
@@ -50518,16 +50685,16 @@
         <v>0</v>
       </c>
       <c r="JQ55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JR55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JS55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JT55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JU55">
         <v>0</v>
@@ -50548,16 +50715,16 @@
         <v>0</v>
       </c>
       <c r="KA55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KB55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KC55">
         <v>0</v>
       </c>
       <c r="KD55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KE55">
         <v>1</v>
@@ -50566,7 +50733,7 @@
         <v>1</v>
       </c>
       <c r="KG55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KH55">
         <v>0</v>
@@ -50583,8 +50750,11 @@
       <c r="KL55">
         <v>0</v>
       </c>
+      <c r="KM55">
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>372</v>
       </c>
@@ -51231,10 +51401,10 @@
         <v>0</v>
       </c>
       <c r="HH56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HI56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HJ56">
         <v>0</v>
@@ -51246,10 +51416,10 @@
         <v>0</v>
       </c>
       <c r="HM56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO56">
         <v>0</v>
@@ -51264,10 +51434,10 @@
         <v>0</v>
       </c>
       <c r="HS56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HU56">
         <v>0</v>
@@ -51276,10 +51446,10 @@
         <v>0</v>
       </c>
       <c r="HW56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY56">
         <v>0</v>
@@ -51291,10 +51461,10 @@
         <v>0</v>
       </c>
       <c r="IB56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IC56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ID56">
         <v>0</v>
@@ -51312,13 +51482,13 @@
         <v>0</v>
       </c>
       <c r="II56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IJ56">
         <v>1</v>
       </c>
       <c r="IK56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IL56">
         <v>0</v>
@@ -51348,22 +51518,22 @@
         <v>0</v>
       </c>
       <c r="IU56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IV56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IW56">
         <v>0</v>
       </c>
       <c r="IX56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IY56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IZ56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JA56">
         <v>1</v>
@@ -51372,7 +51542,7 @@
         <v>1</v>
       </c>
       <c r="JC56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD56">
         <v>0</v>
@@ -51432,10 +51602,10 @@
         <v>0</v>
       </c>
       <c r="JW56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JX56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JY56">
         <v>0</v>
@@ -51444,25 +51614,25 @@
         <v>0</v>
       </c>
       <c r="KA56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KB56">
         <v>1</v>
       </c>
       <c r="KC56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KD56">
         <v>0</v>
       </c>
       <c r="KE56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KF56">
         <v>1</v>
       </c>
       <c r="KG56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KH56">
         <v>0</v>
@@ -51479,8 +51649,11 @@
       <c r="KL56">
         <v>0</v>
       </c>
+      <c r="KM56">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>372</v>
       </c>
@@ -52127,10 +52300,10 @@
         <v>0</v>
       </c>
       <c r="HH57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HI57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HJ57">
         <v>0</v>
@@ -52172,10 +52345,10 @@
         <v>0</v>
       </c>
       <c r="HW57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HX57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HY57">
         <v>0</v>
@@ -52244,13 +52417,13 @@
         <v>0</v>
       </c>
       <c r="IU57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IV57">
         <v>1</v>
       </c>
       <c r="IW57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IX57">
         <v>0</v>
@@ -52262,10 +52435,10 @@
         <v>0</v>
       </c>
       <c r="JA57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JB57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JC57">
         <v>0</v>
@@ -52355,10 +52528,10 @@
         <v>0</v>
       </c>
       <c r="KF57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KG57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KH57">
         <v>0</v>
@@ -52375,8 +52548,11 @@
       <c r="KL57">
         <v>0</v>
       </c>
+      <c r="KM57">
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>373</v>
       </c>
@@ -53038,10 +53214,10 @@
         <v>0</v>
       </c>
       <c r="HM58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO58">
         <v>0</v>
@@ -53083,10 +53259,10 @@
         <v>0</v>
       </c>
       <c r="IB58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IC58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ID58">
         <v>0</v>
@@ -53098,10 +53274,10 @@
         <v>0</v>
       </c>
       <c r="IG58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II58">
         <v>0</v>
@@ -53161,10 +53337,10 @@
         <v>0</v>
       </c>
       <c r="JB58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD58">
         <v>0</v>
@@ -53271,8 +53447,11 @@
       <c r="KL58">
         <v>0</v>
       </c>
+      <c r="KM58">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>373</v>
       </c>
@@ -53934,10 +54113,10 @@
         <v>0</v>
       </c>
       <c r="HM59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO59">
         <v>0</v>
@@ -54057,10 +54236,10 @@
         <v>0</v>
       </c>
       <c r="JB59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD59">
         <v>0</v>
@@ -54167,8 +54346,11 @@
       <c r="KL59">
         <v>0</v>
       </c>
+      <c r="KM59">
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:298" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:299" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>373</v>
       </c>
@@ -54830,10 +55012,10 @@
         <v>0</v>
       </c>
       <c r="HM60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HN60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HO60">
         <v>0</v>
@@ -54875,10 +55057,10 @@
         <v>0</v>
       </c>
       <c r="IB60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IC60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ID60">
         <v>0</v>
@@ -54890,10 +55072,10 @@
         <v>0</v>
       </c>
       <c r="IG60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="IH60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II60">
         <v>0</v>
@@ -54953,10 +55135,10 @@
         <v>0</v>
       </c>
       <c r="JB60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JC60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD60">
         <v>0</v>
@@ -54965,10 +55147,10 @@
         <v>0</v>
       </c>
       <c r="JF60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="JG60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JH60">
         <v>0</v>
@@ -55040,10 +55222,10 @@
         <v>0</v>
       </c>
       <c r="KE60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="KF60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KG60">
         <v>0</v>
@@ -55061,13 +55243,16 @@
         <v>0</v>
       </c>
       <c r="KL60">
+        <v>0</v>
+      </c>
+      <c r="KM60">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:KL60"/>
+  <autoFilter ref="A3:KM60"/>
   <mergeCells count="3">
-    <mergeCell ref="DI1:KL1"/>
+    <mergeCell ref="DI1:KM1"/>
     <mergeCell ref="CG1:DH1"/>
     <mergeCell ref="D1:CF1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Update functions & vignettes; Remove archive
</commit_message>
<xml_diff>
--- a/data-raw/functionsTracker_20230710.xlsx
+++ b/data-raw/functionsTracker_20230710.xlsx
@@ -1819,10 +1819,10 @@
   <dimension ref="A1:KV61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="GY4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="GY19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="HD5" sqref="HD5"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26177,7 +26177,7 @@
         <v>364</v>
       </c>
       <c r="B28" t="s">
-        <v>459</v>
+        <v>470</v>
       </c>
       <c r="C28" t="s">
         <v>468</v>
@@ -28017,7 +28017,7 @@
         <v>368</v>
       </c>
       <c r="B30" t="s">
-        <v>459</v>
+        <v>470</v>
       </c>
       <c r="C30" t="s">
         <v>468</v>

</xml_diff>